<commit_message>
all updates and testing also completed😋😋😋😋😋
</commit_message>
<xml_diff>
--- a/import-foodproducts-excel/sample.xlsx
+++ b/import-foodproducts-excel/sample.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A78334-EE0A-4043-A7FB-1ED164B3176A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="1335" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -51,19 +50,13 @@
     <t>Dosa</t>
   </si>
   <si>
-    <t xml:space="preserve"> Idly</t>
-  </si>
-  <si>
-    <t>Fried Rice</t>
-  </si>
-  <si>
-    <t>pcs</t>
+    <t>chappathi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,14 +100,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -395,16 +385,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
@@ -434,85 +423,48 @@
         <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>150</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="C3" s="2">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
-        <v>3</v>
+      <c r="E3" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="D9" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>